<commit_message>
updated the data sheets
</commit_message>
<xml_diff>
--- a/concert-data/concert_sheet.xlsx
+++ b/concert-data/concert_sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankek\Documents\Concert Wrapped\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankek\Documents\Concert Wrapped\concert-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{22040B26-256F-47EB-B4C0-EB054315ACD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C39A0A-6304-4681-A61E-F6F0B3802DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A1B8166-E455-4E9D-B974-4CF7D696C47E}"/>
   </bookViews>
@@ -242,9 +242,6 @@
     <t>Companions</t>
   </si>
   <si>
-    <t>Alicia Riss, Nadine Müller</t>
-  </si>
-  <si>
     <t>Daniela Wolfangel</t>
   </si>
   <si>
@@ -254,25 +251,28 @@
     <t>Alica Riss</t>
   </si>
   <si>
-    <t>Daniela Wolfangel, Lisa Schmidt</t>
-  </si>
-  <si>
     <t>Lisa Schmidt</t>
   </si>
   <si>
     <t>Thea Pagel</t>
   </si>
   <si>
-    <t>Martin Kabierski, Daniela Wolfangel, Nina, Nicky</t>
-  </si>
-  <si>
-    <t>Nils Deuermeier, Deborah Budde, Nadine Müller, Marvin Deuermeier, Paddy</t>
-  </si>
-  <si>
     <t>Raja Kabierski</t>
   </si>
   <si>
     <t>Amount of Songs on the Set List</t>
+  </si>
+  <si>
+    <t>Nils Deuermeier; Deborah Budde; Nadine Müller; Marvin Deuermeier; Paddy</t>
+  </si>
+  <si>
+    <t>Martin Kabierski; Daniela Wolfangel; Nina; Nicky</t>
+  </si>
+  <si>
+    <t>Daniela Wolfangel; Lisa Schmidt</t>
+  </si>
+  <si>
+    <t>Alicia Riss; Nadine Müller</t>
   </si>
 </sst>
 </file>
@@ -649,7 +649,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +694,7 @@
         <v>67</v>
       </c>
       <c r="J1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -723,7 +723,7 @@
         <v>64</v>
       </c>
       <c r="I2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="J2">
         <v>19</v>
@@ -755,7 +755,7 @@
         <v>64</v>
       </c>
       <c r="I3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -781,7 +781,7 @@
         <v>65</v>
       </c>
       <c r="I4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J4">
         <v>19</v>
@@ -813,7 +813,7 @@
         <v>64</v>
       </c>
       <c r="I5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J5">
         <v>20</v>
@@ -845,7 +845,7 @@
         <v>64</v>
       </c>
       <c r="I6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J6">
         <v>22</v>
@@ -909,7 +909,7 @@
         <v>64</v>
       </c>
       <c r="I8" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="J8">
         <v>20</v>
@@ -941,7 +941,7 @@
         <v>64</v>
       </c>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J9">
         <v>22</v>
@@ -973,7 +973,7 @@
         <v>64</v>
       </c>
       <c r="I10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J10">
         <v>18</v>
@@ -1005,7 +1005,7 @@
         <v>64</v>
       </c>
       <c r="I11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1034,7 +1034,7 @@
         <v>64</v>
       </c>
       <c r="I12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J12">
         <v>15</v>
@@ -1066,7 +1066,7 @@
         <v>64</v>
       </c>
       <c r="I13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J13">
         <v>17</v>
@@ -1127,7 +1127,7 @@
         <v>64</v>
       </c>
       <c r="I15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J15">
         <v>22</v>
@@ -1159,7 +1159,7 @@
         <v>64</v>
       </c>
       <c r="I16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J16">
         <v>30</v>
@@ -1191,7 +1191,7 @@
         <v>64</v>
       </c>
       <c r="I17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1292,7 +1292,7 @@
         <v>64</v>
       </c>
       <c r="I21" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1318,7 +1318,7 @@
         <v>64</v>
       </c>
       <c r="I22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data Sheet update coordinates for locations
</commit_message>
<xml_diff>
--- a/concert-data/concert_sheet.xlsx
+++ b/concert-data/concert_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankek\Documents\Concert Wrapped\concert-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C39A0A-6304-4681-A61E-F6F0B3802DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{34D73AD3-CD62-47C0-92DB-09028C250716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A1B8166-E455-4E9D-B974-4CF7D696C47E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="117">
   <si>
     <t>Artist</t>
   </si>
@@ -273,6 +273,120 @@
   </si>
   <si>
     <t>Alicia Riss; Nadine Müller</t>
+  </si>
+  <si>
+    <t>Location Latitude</t>
+  </si>
+  <si>
+    <t>Location Longitude</t>
+  </si>
+  <si>
+    <t>50.96935015828385</t>
+  </si>
+  <si>
+    <t>7.016967748530129</t>
+  </si>
+  <si>
+    <t>13.413732005431044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52.539476472121635 </t>
+  </si>
+  <si>
+    <t>13.392419127117439</t>
+  </si>
+  <si>
+    <t>52.48465166325178</t>
+  </si>
+  <si>
+    <t>13.44380326237846</t>
+  </si>
+  <si>
+    <t>52.50656898406912</t>
+  </si>
+  <si>
+    <t>52.31368972777124</t>
+  </si>
+  <si>
+    <t>4.937152491925177</t>
+  </si>
+  <si>
+    <t>50.888175749540146</t>
+  </si>
+  <si>
+    <t>5.981013584448024</t>
+  </si>
+  <si>
+    <t>13.38123873571791</t>
+  </si>
+  <si>
+    <t>52.501750034103296</t>
+  </si>
+  <si>
+    <t>52.49939608591923</t>
+  </si>
+  <si>
+    <t>13.445110926676438</t>
+  </si>
+  <si>
+    <t>52.51566105735034</t>
+  </si>
+  <si>
+    <t>13.229304057727013</t>
+  </si>
+  <si>
+    <t>52.50743939996307</t>
+  </si>
+  <si>
+    <t>13.454763080229027</t>
+  </si>
+  <si>
+    <t>52.5308904332696</t>
+  </si>
+  <si>
+    <t>13.451074492408171</t>
+  </si>
+  <si>
+    <t>52.03158665845571</t>
+  </si>
+  <si>
+    <t>8.516188994603466</t>
+  </si>
+  <si>
+    <t>52.54022009347248</t>
+  </si>
+  <si>
+    <t>13.212430995650017</t>
+  </si>
+  <si>
+    <t>52.47707236704825</t>
+  </si>
+  <si>
+    <t>13.439662645360936</t>
+  </si>
+  <si>
+    <t>52.47921993518094</t>
+  </si>
+  <si>
+    <t>13.438878566152086</t>
+  </si>
+  <si>
+    <t>52.50784702854427</t>
+  </si>
+  <si>
+    <t>13.451965957743411</t>
+  </si>
+  <si>
+    <t>52.505330131885934</t>
+  </si>
+  <si>
+    <t>13.443831592329605</t>
+  </si>
+  <si>
+    <t>51.89778511192236</t>
+  </si>
+  <si>
+    <t>4.493796148615386</t>
   </si>
 </sst>
 </file>
@@ -308,10 +422,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,26 +761,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0C6205-7210-4334-A696-6AB2F5EDFFAF}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="9" width="67.28515625" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" customWidth="1"/>
+    <col min="5" max="7" width="30.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="11" max="11" width="67.28515625" customWidth="1"/>
+    <col min="12" max="12" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -678,26 +791,32 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>63</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>67</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -710,26 +829,32 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>4000</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2">
+      <c r="I2" s="1">
         <v>45340</v>
       </c>
-      <c r="H2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" t="s">
         <v>78</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -742,23 +867,29 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>1000</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2">
+      <c r="I3" s="1">
         <v>45342</v>
       </c>
-      <c r="H3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -768,26 +899,32 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>3500</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="2">
+      <c r="I4" s="1">
         <v>45343</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>65</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>68</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -800,26 +937,32 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>17000</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2">
+      <c r="I5" s="1">
         <v>45362</v>
       </c>
-      <c r="H5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" t="s">
         <v>69</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -832,26 +975,32 @@
       <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="3">
         <v>17000</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="2">
+      <c r="I6" s="1">
         <v>45378</v>
       </c>
-      <c r="H6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" t="s">
         <v>70</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -864,26 +1013,32 @@
       <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>600</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="2">
+      <c r="I7" s="1">
         <v>45380</v>
       </c>
-      <c r="H7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" t="s">
         <v>66</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -896,26 +1051,32 @@
       <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>1000</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="2">
+      <c r="I8" s="1">
         <v>45389</v>
       </c>
-      <c r="H8" t="s">
-        <v>64</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" t="s">
         <v>77</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -928,26 +1089,32 @@
       <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>4200</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="2">
+      <c r="I9" s="1">
         <v>45402</v>
       </c>
-      <c r="H9" t="s">
-        <v>64</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" t="s">
         <v>68</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -960,26 +1127,32 @@
       <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>4000</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="2">
+      <c r="I10" s="1">
         <v>45422</v>
       </c>
-      <c r="H10" t="s">
-        <v>64</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" t="s">
         <v>71</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -992,23 +1165,29 @@
       <c r="D11" t="s">
         <v>10</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>4200</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="2">
+      <c r="I11" s="1">
         <v>45429</v>
       </c>
-      <c r="H11" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1021,26 +1200,32 @@
       <c r="D12" t="s">
         <v>10</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>600</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="2">
+      <c r="I12" s="1">
         <v>45442</v>
       </c>
-      <c r="H12" t="s">
-        <v>64</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
+        <v>64</v>
+      </c>
+      <c r="K12" t="s">
         <v>72</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1053,26 +1238,32 @@
       <c r="D13" t="s">
         <v>10</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>22290</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="2">
+      <c r="I13" s="1">
         <v>45448</v>
       </c>
-      <c r="H13" t="s">
-        <v>64</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
+        <v>64</v>
+      </c>
+      <c r="K13" t="s">
         <v>76</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1085,23 +1276,29 @@
       <c r="D14" t="s">
         <v>10</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>270</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="2">
+      <c r="I14" s="1">
         <v>45449</v>
       </c>
-      <c r="H14" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14">
+      <c r="J14" t="s">
+        <v>64</v>
+      </c>
+      <c r="L14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -1114,26 +1311,32 @@
       <c r="D15" t="s">
         <v>10</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>12000</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H15" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="2">
+      <c r="I15" s="1">
         <v>45454</v>
       </c>
-      <c r="H15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
+        <v>64</v>
+      </c>
+      <c r="K15" t="s">
         <v>68</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1146,26 +1349,32 @@
       <c r="D16" t="s">
         <v>42</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>28000</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H16" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="2">
+      <c r="I16" s="1">
         <v>45458</v>
       </c>
-      <c r="H16" t="s">
-        <v>64</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
+        <v>64</v>
+      </c>
+      <c r="K16" t="s">
         <v>75</v>
       </c>
-      <c r="J16">
+      <c r="L16">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1178,23 +1387,29 @@
       <c r="D17" t="s">
         <v>10</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>10000</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H17" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="2">
+      <c r="I17" s="1">
         <v>45531</v>
       </c>
-      <c r="H17" t="s">
-        <v>64</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
+        <v>64</v>
+      </c>
+      <c r="K17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1207,20 +1422,26 @@
       <c r="D18" t="s">
         <v>10</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>254</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H18" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="2">
+      <c r="I18" s="1">
         <v>45546</v>
       </c>
-      <c r="H18" t="s">
+      <c r="J18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -1230,20 +1451,26 @@
       <c r="D19" t="s">
         <v>10</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>250</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H19" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="2">
+      <c r="I19" s="1">
         <v>45555</v>
       </c>
-      <c r="H19" t="s">
+      <c r="J19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -1256,20 +1483,26 @@
       <c r="D20" t="s">
         <v>10</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>1500</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" t="s">
         <v>55</v>
       </c>
-      <c r="G20" s="2">
+      <c r="I20" s="1">
         <v>45588</v>
       </c>
-      <c r="H20" t="s">
+      <c r="J20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -1279,23 +1512,29 @@
       <c r="D21" t="s">
         <v>10</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>4500</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H21" t="s">
         <v>57</v>
       </c>
-      <c r="G21" s="2">
+      <c r="I21" s="1">
         <v>45582</v>
       </c>
-      <c r="H21" t="s">
-        <v>64</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
+        <v>64</v>
+      </c>
+      <c r="K21" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1305,23 +1544,30 @@
       <c r="D22" t="s">
         <v>58</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>4000</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H22" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="2">
+      <c r="I22" s="1">
         <v>45595</v>
       </c>
-      <c r="H22" t="s">
-        <v>64</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
+        <v>64</v>
+      </c>
+      <c r="K22" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Getting total number of concerts through concertId column
</commit_message>
<xml_diff>
--- a/concert-data/concert_sheet.xlsx
+++ b/concert-data/concert_sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankek\Documents\Concert Wrapped\concert-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34D73AD3-CD62-47C0-92DB-09028C250716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A618213-964A-4338-80BD-26070082F0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A1B8166-E455-4E9D-B974-4CF7D696C47E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="118">
   <si>
     <t>Artist</t>
   </si>
@@ -197,15 +197,6 @@
     <t>Prachtwerk</t>
   </si>
   <si>
-    <t>Chance Pena</t>
-  </si>
-  <si>
-    <t>Jonah Kagen</t>
-  </si>
-  <si>
-    <t>Astra Kulturhaus</t>
-  </si>
-  <si>
     <t>Lizzy McAlpine</t>
   </si>
   <si>
@@ -371,12 +362,6 @@
     <t>13.438878566152086</t>
   </si>
   <si>
-    <t>52.50784702854427</t>
-  </si>
-  <si>
-    <t>13.451965957743411</t>
-  </si>
-  <si>
     <t>52.505330131885934</t>
   </si>
   <si>
@@ -387,6 +372,24 @@
   </si>
   <si>
     <t>4.493796148615386</t>
+  </si>
+  <si>
+    <t>Chappell Roan</t>
+  </si>
+  <si>
+    <t>12000</t>
+  </si>
+  <si>
+    <t>Peter Fox</t>
+  </si>
+  <si>
+    <t>Görlitzer Park</t>
+  </si>
+  <si>
+    <t>52.49678216757308</t>
+  </si>
+  <si>
+    <t>13.437405995049385</t>
   </si>
 </sst>
 </file>
@@ -761,9 +764,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0C6205-7210-4334-A696-6AB2F5EDFFAF}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -786,7 +791,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -795,10 +800,10 @@
         <v>44</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -807,13 +812,13 @@
         <v>45</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -824,7 +829,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -833,10 +838,10 @@
         <v>4000</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H2" t="s">
         <v>7</v>
@@ -845,10 +850,10 @@
         <v>45340</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L2">
         <v>19</v>
@@ -862,7 +867,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -871,10 +876,10 @@
         <v>1000</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
@@ -883,10 +888,10 @@
         <v>45342</v>
       </c>
       <c r="J3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -894,7 +899,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -903,10 +908,10 @@
         <v>3500</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
@@ -915,10 +920,10 @@
         <v>45343</v>
       </c>
       <c r="J4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" t="s">
         <v>65</v>
-      </c>
-      <c r="K4" t="s">
-        <v>68</v>
       </c>
       <c r="L4">
         <v>19</v>
@@ -932,7 +937,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -941,10 +946,10 @@
         <v>17000</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -953,10 +958,10 @@
         <v>45362</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L5">
         <v>20</v>
@@ -970,7 +975,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -979,10 +984,10 @@
         <v>17000</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H6" t="s">
         <v>17</v>
@@ -991,10 +996,10 @@
         <v>45378</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L6">
         <v>22</v>
@@ -1008,7 +1013,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -1017,10 +1022,10 @@
         <v>600</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H7" t="s">
         <v>19</v>
@@ -1029,10 +1034,10 @@
         <v>45380</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L7">
         <v>18</v>
@@ -1046,7 +1051,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -1055,10 +1060,10 @@
         <v>1000</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H8" t="s">
         <v>11</v>
@@ -1067,10 +1072,10 @@
         <v>45389</v>
       </c>
       <c r="J8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L8">
         <v>20</v>
@@ -1084,7 +1089,7 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -1093,10 +1098,10 @@
         <v>4200</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H9" t="s">
         <v>24</v>
@@ -1105,10 +1110,10 @@
         <v>45402</v>
       </c>
       <c r="J9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L9">
         <v>22</v>
@@ -1122,7 +1127,7 @@
         <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
@@ -1131,10 +1136,10 @@
         <v>4000</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H10" t="s">
         <v>7</v>
@@ -1143,10 +1148,10 @@
         <v>45422</v>
       </c>
       <c r="J10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L10">
         <v>18</v>
@@ -1160,7 +1165,7 @@
         <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -1169,10 +1174,10 @@
         <v>4200</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H11" t="s">
         <v>24</v>
@@ -1181,10 +1186,10 @@
         <v>45429</v>
       </c>
       <c r="J11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1195,7 +1200,7 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -1204,10 +1209,10 @@
         <v>600</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -1216,10 +1221,10 @@
         <v>45442</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L12">
         <v>15</v>
@@ -1233,7 +1238,7 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -1242,10 +1247,10 @@
         <v>22290</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H13" t="s">
         <v>34</v>
@@ -1254,10 +1259,10 @@
         <v>45448</v>
       </c>
       <c r="J13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L13">
         <v>17</v>
@@ -1271,7 +1276,7 @@
         <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -1280,10 +1285,10 @@
         <v>270</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H14" t="s">
         <v>36</v>
@@ -1292,7 +1297,7 @@
         <v>45449</v>
       </c>
       <c r="J14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L14">
         <v>12</v>
@@ -1306,7 +1311,7 @@
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
@@ -1315,10 +1320,10 @@
         <v>12000</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H15" t="s">
         <v>39</v>
@@ -1327,10 +1332,10 @@
         <v>45454</v>
       </c>
       <c r="J15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L15">
         <v>22</v>
@@ -1344,7 +1349,7 @@
         <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
         <v>42</v>
@@ -1353,10 +1358,10 @@
         <v>28000</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H16" t="s">
         <v>43</v>
@@ -1365,10 +1370,10 @@
         <v>45458</v>
       </c>
       <c r="J16" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L16">
         <v>30</v>
@@ -1382,7 +1387,7 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
@@ -1391,10 +1396,10 @@
         <v>10000</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H17" t="s">
         <v>47</v>
@@ -1403,10 +1408,10 @@
         <v>45531</v>
       </c>
       <c r="J17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1417,7 +1422,7 @@
         <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
@@ -1426,10 +1431,10 @@
         <v>254</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H18" t="s">
         <v>50</v>
@@ -1438,7 +1443,7 @@
         <v>45546</v>
       </c>
       <c r="J18" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1446,7 +1451,7 @@
         <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
@@ -1455,10 +1460,10 @@
         <v>250</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H19" t="s">
         <v>52</v>
@@ -1467,103 +1472,135 @@
         <v>45555</v>
       </c>
       <c r="J19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="2">
-        <v>1500</v>
+      <c r="E20" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H20" t="s">
-        <v>55</v>
+        <v>99</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="I20" s="1">
         <v>45588</v>
       </c>
       <c r="J20" t="s">
+        <v>61</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="2">
-        <v>4500</v>
+      <c r="E21" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H21" t="s">
-        <v>57</v>
+        <v>117</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="I21" s="1">
-        <v>45582</v>
+        <v>45556</v>
       </c>
       <c r="J21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2">
+        <v>4500</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" s="1">
+        <v>45582</v>
+      </c>
+      <c r="J22" t="s">
+        <v>61</v>
+      </c>
+      <c r="K22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>8</v>
       </c>
-      <c r="C22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="2">
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="2">
         <v>4000</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H22" t="s">
-        <v>59</v>
-      </c>
-      <c r="I22" s="1">
+      <c r="F23" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="1">
         <v>45595</v>
       </c>
-      <c r="J22" t="s">
-        <v>64</v>
-      </c>
-      <c r="K22" t="s">
-        <v>71</v>
+      <c r="J23" t="s">
+        <v>61</v>
+      </c>
+      <c r="K23" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>